<commit_message>
Update to TEST Template file
</commit_message>
<xml_diff>
--- a/TEST.xlsx
+++ b/TEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedan\Documents\Masters\NEU\RA\SmeLLM\Github\SmeLLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DF114-1121-4DFB-BD84-289A134EACB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F457DD4-37FA-4680-BD46-7A42B1D8A10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
   <si>
     <t>File Name</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>TFGE1</t>
+  </si>
+  <si>
+    <t>DCLSGE1</t>
   </si>
 </sst>
 </file>
@@ -393,11 +396,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,7 +707,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G70"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,114 +726,114 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
+      <c r="A10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final updates to TEST.xlsx template
</commit_message>
<xml_diff>
--- a/TEST.xlsx
+++ b/TEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedan\Documents\Masters\NEU\RA\SmeLLM\Github\SmeLLM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F457DD4-37FA-4680-BD46-7A42B1D8A10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6FE2EE-AD45-4034-8EB0-9CB7C0BD952E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>File Name</t>
   </si>
@@ -169,9 +169,6 @@
     <t>LCGE1</t>
   </si>
   <si>
-    <t>["'Primitive Obsession"]</t>
-  </si>
-  <si>
     <t>LCGE2</t>
   </si>
   <si>
@@ -301,9 +298,6 @@
     <t>SSBE1</t>
   </si>
   <si>
-    <t>["'Shotgun Surgery", "'Feature Envy'", "'Duplicate Code'", "'Primitive Obsession'", "'Alternative Classes with Different Interfaces'"]</t>
-  </si>
-  <si>
     <t>SSGE1</t>
   </si>
   <si>
@@ -341,6 +335,9 @@
   </si>
   <si>
     <t>DCLSGE1</t>
+  </si>
+  <si>
+    <t>['Shotgun Surgery', 'Feature Envy', 'Duplicate Code', 'Primitive Obsession','Alternative Classes with Different Interfaces']</t>
   </si>
 </sst>
 </file>
@@ -706,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B70" sqref="A2:B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,7 +788,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
@@ -838,442 +835,442 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>63</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>70</v>
-      </c>
-      <c r="B45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>72</v>
-      </c>
-      <c r="B47" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>84</v>
-      </c>
-      <c r="B55" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>86</v>
-      </c>
-      <c r="B56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>89</v>
-      </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>96</v>
-      </c>
-      <c r="B63" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="B66" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B65" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="B67" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B66" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="B68" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B67" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="B69" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B68" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B69" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>105</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>